<commit_message>
changes for class presentation of syllabus
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -195,9 +195,6 @@
     <t>Lecture</t>
   </si>
   <si>
-    <t>Topic and Timeline</t>
-  </si>
-  <si>
     <t>NPV IRR</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>Outline Feedback</t>
   </si>
   <si>
-    <t>article and discussion</t>
-  </si>
-  <si>
     <t>Activity</t>
   </si>
   <si>
@@ -291,18 +285,6 @@
     <t>Quiz 7</t>
   </si>
   <si>
-    <t>Homework 1 Due</t>
-  </si>
-  <si>
-    <t>Homework 2 Due</t>
-  </si>
-  <si>
-    <t>Homework 3 Due</t>
-  </si>
-  <si>
-    <t>Homework 4 Due</t>
-  </si>
-  <si>
     <t>REEPS 2.1-2.2</t>
   </si>
   <si>
@@ -337,6 +319,24 @@
   </si>
   <si>
     <t>2013-10-13-three phase</t>
+  </si>
+  <si>
+    <t>Homework 5</t>
+  </si>
+  <si>
+    <t>Homework 4</t>
+  </si>
+  <si>
+    <t>Homework 3</t>
+  </si>
+  <si>
+    <t>Homework 2</t>
+  </si>
+  <si>
+    <t>Homework 1</t>
+  </si>
+  <si>
+    <t>Choose topic</t>
   </si>
 </sst>
 </file>
@@ -396,8 +396,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -514,7 +532,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -565,6 +583,15 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -615,6 +642,15 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -947,7 +983,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -973,13 +1009,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1012,14 +1048,8 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1">
@@ -1033,10 +1063,16 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1">
@@ -1047,13 +1083,13 @@
         <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1">
@@ -1067,13 +1103,10 @@
         <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1">
@@ -1084,13 +1117,10 @@
         <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1">
@@ -1101,13 +1131,16 @@
         <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1">
@@ -1118,10 +1151,10 @@
         <v>35</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1">
@@ -1132,7 +1165,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1">
@@ -1143,13 +1176,13 @@
         <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1">
@@ -1160,16 +1193,19 @@
         <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1">
@@ -1183,10 +1219,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1">
@@ -1200,10 +1233,13 @@
         <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1">
@@ -1214,10 +1250,10 @@
         <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1">
@@ -1228,7 +1264,10 @@
         <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1">
@@ -1242,7 +1281,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1">
@@ -1255,9 +1294,6 @@
       <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1">
       <c r="A19" s="2">
@@ -1269,9 +1305,6 @@
       <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="20" spans="1:8" ht="18" customHeight="1">
       <c r="A20" s="2">
@@ -1284,13 +1317,19 @@
         <v>17</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18" customHeight="1">
@@ -1332,10 +1371,10 @@
         <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" customHeight="1">
@@ -1349,13 +1388,13 @@
         <v>21</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" customHeight="1">
@@ -1366,7 +1405,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18" customHeight="1">
@@ -1377,7 +1416,7 @@
         <v>52</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18" customHeight="1">
@@ -1388,10 +1427,7 @@
         <v>53</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>23</v>
@@ -1432,17 +1468,17 @@
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1">
       <c r="D31" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1">
       <c r="D32" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="18" customHeight="1">
       <c r="D33" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revises reading due dates
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25220" windowHeight="28360" tabRatio="793"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="793"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
   <si>
     <t>Date</t>
   </si>
@@ -285,12 +285,6 @@
     <t>Quiz 7</t>
   </si>
   <si>
-    <t>REEPS 2.1-2.2</t>
-  </si>
-  <si>
-    <t>REEPS 2.3-2.4</t>
-  </si>
-  <si>
     <t>REEPS 2.4-2.8</t>
   </si>
   <si>
@@ -337,6 +331,9 @@
   </si>
   <si>
     <t>Choose topic</t>
+  </si>
+  <si>
+    <t>REEPS 2.1-2.4</t>
   </si>
 </sst>
 </file>
@@ -983,7 +980,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1048,9 +1045,6 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1">
       <c r="A4" s="2">
@@ -1069,7 +1063,7 @@
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>26</v>
@@ -1140,7 +1134,7 @@
         <v>82</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1">
@@ -1154,7 +1148,7 @@
         <v>60</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1">
@@ -1176,13 +1170,13 @@
         <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>83</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1">
@@ -1193,16 +1187,16 @@
         <v>38</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>61</v>
@@ -1236,7 +1230,7 @@
         <v>84</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>63</v>
@@ -1267,7 +1261,7 @@
         <v>62</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1">
@@ -1323,7 +1317,7 @@
         <v>86</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>5</v>
@@ -1374,7 +1368,7 @@
         <v>87</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" customHeight="1">
@@ -1391,7 +1385,7 @@
         <v>70</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>75</v>
@@ -1416,7 +1410,7 @@
         <v>52</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18" customHeight="1">
@@ -1427,7 +1421,7 @@
         <v>53</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>23</v>
@@ -1468,17 +1462,17 @@
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1">
       <c r="D31" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1">
       <c r="D32" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="18" customHeight="1">
       <c r="D33" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
date changes on syllabus
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -39,15 +39,9 @@
     <t>REEPS2 Appendix A</t>
   </si>
   <si>
-    <t>REEPS2 Chapter 3</t>
-  </si>
-  <si>
     <t>Presentations</t>
   </si>
   <si>
-    <t>Luenberger</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -246,9 +240,6 @@
     <t>ipynb AC demonstrations</t>
   </si>
   <si>
-    <t>REEPS 1</t>
-  </si>
-  <si>
     <t>Kirchoff's Laws</t>
   </si>
   <si>
@@ -330,10 +321,22 @@
     <t>Homework 1</t>
   </si>
   <si>
-    <t>Choose topic</t>
-  </si>
-  <si>
     <t>REEPS 2.1-2.4</t>
+  </si>
+  <si>
+    <t>REEPS 3.4</t>
+  </si>
+  <si>
+    <t>REEPS 3.5</t>
+  </si>
+  <si>
+    <t>REEPS 1, 3.7</t>
+  </si>
+  <si>
+    <t>Luenberger 2</t>
+  </si>
+  <si>
+    <t>LBNL Reading</t>
   </si>
 </sst>
 </file>
@@ -393,8 +396,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -529,7 +534,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="121">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -589,6 +594,7 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -648,6 +654,7 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -979,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1000,19 +1007,19 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -1021,7 +1028,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" customHeight="1">
@@ -1029,7 +1036,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1040,10 +1047,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18" customHeight="1">
@@ -1051,22 +1058,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1">
@@ -1074,16 +1078,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1">
@@ -1091,16 +1095,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1">
@@ -1108,13 +1112,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1">
@@ -1122,19 +1129,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1">
@@ -1142,13 +1149,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1">
@@ -1156,10 +1160,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1">
@@ -1167,16 +1174,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1">
@@ -1184,22 +1191,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1">
@@ -1207,13 +1214,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1">
@@ -1221,19 +1228,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1">
@@ -1241,13 +1248,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1">
@@ -1255,13 +1265,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1">
@@ -1269,13 +1279,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1">
@@ -1283,10 +1296,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1">
@@ -1294,10 +1307,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18" customHeight="1">
@@ -1305,25 +1318,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18" customHeight="1">
@@ -1331,10 +1344,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" customHeight="1">
@@ -1342,16 +1355,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18" customHeight="1">
@@ -1359,16 +1369,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" customHeight="1">
@@ -1376,19 +1386,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" customHeight="1">
@@ -1396,10 +1406,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18" customHeight="1">
@@ -1407,10 +1417,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18" customHeight="1">
@@ -1418,13 +1428,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18" customHeight="1">
@@ -1432,10 +1442,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18" customHeight="1">
@@ -1443,10 +1453,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18" customHeight="1">
@@ -1454,25 +1464,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1">
       <c r="D31" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1">
       <c r="D32" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="18" customHeight="1">
       <c r="D33" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates syllabus for meier reading
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16780" windowHeight="19960" tabRatio="793"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14740" tabRatio="793"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
   <si>
     <t>Date</t>
   </si>
@@ -252,24 +252,6 @@
     <t>Quiz 1</t>
   </si>
   <si>
-    <t>Quiz 2</t>
-  </si>
-  <si>
-    <t>Quiz 3</t>
-  </si>
-  <si>
-    <t>Quiz 4</t>
-  </si>
-  <si>
-    <t>Quiz 5</t>
-  </si>
-  <si>
-    <t>Quiz 6</t>
-  </si>
-  <si>
-    <t>Quiz 7</t>
-  </si>
-  <si>
     <t>REEPS 2.4-2.8</t>
   </si>
   <si>
@@ -327,9 +309,6 @@
     <t>REEPS 1, 3.7</t>
   </si>
   <si>
-    <t>LBNL Reading</t>
-  </si>
-  <si>
     <t>Ohm and Kirchoff Laws</t>
   </si>
   <si>
@@ -337,6 +316,9 @@
   </si>
   <si>
     <t>Luenberger 1-2</t>
+  </si>
+  <si>
+    <t>Meier, 1984</t>
   </si>
 </sst>
 </file>
@@ -986,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1061,7 +1043,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>62</v>
@@ -1070,7 +1052,7 @@
         <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1">
@@ -1081,13 +1063,10 @@
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1">
@@ -1104,7 +1083,7 @@
         <v>63</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18" customHeight="1">
@@ -1137,11 +1116,8 @@
       <c r="D8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="F8" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1">
@@ -1165,8 +1141,11 @@
       <c r="C10" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="E10" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="G10" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" customHeight="1">
@@ -1177,13 +1156,10 @@
         <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1">
@@ -1194,16 +1170,16 @@
         <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>65</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>58</v>
@@ -1233,11 +1209,8 @@
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="G14" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>60</v>
@@ -1257,7 +1230,7 @@
         <v>71</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1">
@@ -1271,7 +1244,7 @@
         <v>59</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1">
@@ -1284,11 +1257,8 @@
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="G17" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1">
@@ -1326,11 +1296,8 @@
       <c r="D20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>4</v>
@@ -1374,11 +1341,8 @@
       <c r="C23" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" customHeight="1">
@@ -1395,10 +1359,10 @@
         <v>67</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" customHeight="1">
@@ -1420,7 +1384,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18" customHeight="1">
@@ -1431,7 +1395,7 @@
         <v>50</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>20</v>
@@ -1472,17 +1436,17 @@
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1">
       <c r="D31" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1">
       <c r="D32" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="18" customHeight="1">
       <c r="D33" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrects error on readings
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14740" tabRatio="793"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="793"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">schedule!$A$1:$F$30</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -252,9 +255,6 @@
     <t>Quiz 1</t>
   </si>
   <si>
-    <t>REEPS 2.4-2.8</t>
-  </si>
-  <si>
     <t>REEPS 3.1-3.2</t>
   </si>
   <si>
@@ -319,13 +319,16 @@
   </si>
   <si>
     <t>Meier, 1984</t>
+  </si>
+  <si>
+    <t>REEPS 2.5-2.8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -360,6 +363,12 @@
       <color rgb="FF000000"/>
       <name val="Courier"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -369,7 +378,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -377,8 +386,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="121">
+  <cellStyleXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -500,8 +546,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -515,8 +565,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="121">
+  <cellStyles count="125">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -577,6 +648,8 @@
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -637,6 +710,8 @@
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -966,10 +1041,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F1" sqref="A1:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -977,483 +1055,549 @@
     <col min="1" max="1" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="4"/>
-    <col min="6" max="6" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="8.83203125" style="3"/>
-    <col min="14" max="14" width="24.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="3"/>
+    <col min="4" max="4" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="4"/>
+    <col min="10" max="11" width="8.83203125" style="3"/>
+    <col min="12" max="12" width="24.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9" ht="18" customHeight="1">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" customHeight="1">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" customHeight="1">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18" customHeight="1">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="I10" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" customHeight="1">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18" customHeight="1">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" customHeight="1">
+      <c r="A17" s="10">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" ht="18" customHeight="1">
+      <c r="A18" s="10">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" ht="18" customHeight="1">
+      <c r="A19" s="10">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" ht="18" customHeight="1">
+      <c r="A20" s="10">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18" customHeight="1">
+      <c r="A21" s="10">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" ht="18" customHeight="1">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18" customHeight="1">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" ht="18" customHeight="1">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18" customHeight="1">
+      <c r="A25" s="10">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:7" ht="18" customHeight="1">
+      <c r="A26" s="10">
         <v>25</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="1:7" ht="18" customHeight="1">
+      <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="18" customHeight="1">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B27" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18" customHeight="1">
+      <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B28" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:7" ht="18" customHeight="1">
+      <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1">
-      <c r="A6" s="2">
+      <c r="B29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D29" s="6"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:7" ht="18" customHeight="1">
+      <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="18" customHeight="1">
-      <c r="A8" s="2">
+      <c r="B30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="18" customHeight="1">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="18" customHeight="1">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" customHeight="1">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18" customHeight="1">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="18" customHeight="1">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="18" customHeight="1">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="18" customHeight="1">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="18" customHeight="1">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="18" customHeight="1">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="18" customHeight="1">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="18" customHeight="1">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="18" customHeight="1">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="18" customHeight="1">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="2" t="s">
+      <c r="D30" s="6"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" ht="18" customHeight="1">
+      <c r="G31" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="18" customHeight="1">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="18" customHeight="1">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="18" customHeight="1">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="18" customHeight="1">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="18" customHeight="1">
-      <c r="A28" s="2">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="18" customHeight="1">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="18" customHeight="1">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="18" customHeight="1">
-      <c r="D31" s="3" t="s">
+    <row r="32" spans="1:7" ht="18" customHeight="1">
+      <c r="G32" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="18" customHeight="1">
-      <c r="D32" s="3" t="s">
+    <row r="33" spans="7:7" ht="18" customHeight="1">
+      <c r="G33" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="4:4" ht="18" customHeight="1">
-      <c r="D33" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
+  <pageSetup scale="79" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
moves homework 2 date and outline feedback
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="793"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -322,6 +322,30 @@
   </si>
   <si>
     <t>REEPS 2.5-2.8</t>
+  </si>
+  <si>
+    <t>Quiz 2</t>
+  </si>
+  <si>
+    <t>Quiz 3</t>
+  </si>
+  <si>
+    <t>Quiz 4</t>
+  </si>
+  <si>
+    <t>Quiz 5</t>
+  </si>
+  <si>
+    <t>Quiz 6</t>
+  </si>
+  <si>
+    <t>Quiz 7</t>
+  </si>
+  <si>
+    <t>Quiz 8</t>
+  </si>
+  <si>
+    <t>Quiz 9</t>
   </si>
 </sst>
 </file>
@@ -370,12 +394,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -424,7 +454,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -550,8 +580,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,9 +604,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -583,11 +616,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="131">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -650,6 +692,9 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -712,6 +757,9 @@
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1047,17 +1095,17 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F30"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="4"/>
     <col min="10" max="11" width="8.83203125" style="3"/>
@@ -1066,22 +1114,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1095,47 +1143,47 @@
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1">
       <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1">
       <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="3" t="s">
         <v>62</v>
       </c>
@@ -1144,15 +1192,15 @@
       <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="3" t="s">
         <v>64</v>
       </c>
@@ -1161,17 +1209,17 @@
       <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="3" t="s">
         <v>63</v>
       </c>
@@ -1180,15 +1228,15 @@
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="11" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -1199,17 +1247,17 @@
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
       <c r="G8" s="3" t="s">
         <v>70</v>
       </c>
@@ -1218,68 +1266,65 @@
       <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1">
       <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="I10" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1">
       <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="I11" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="13" t="s">
         <v>58</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -1287,301 +1332,326 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="I13" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="E14" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="11"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="I15" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>88</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:7" ht="18" customHeight="1">
-      <c r="A17" s="10">
+      <c r="F16" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" customHeight="1">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1">
-      <c r="A18" s="10">
+      <c r="F17" s="13"/>
+      <c r="I17" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" customHeight="1">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="11"/>
-    </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1">
-      <c r="A19" s="10">
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" customHeight="1">
+      <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1">
-      <c r="A20" s="10">
+      <c r="F19" s="13"/>
+      <c r="I19" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" customHeight="1">
+      <c r="A20" s="9">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>87</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="13" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1">
-      <c r="A21" s="10">
+    <row r="21" spans="1:9" ht="18" customHeight="1">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="6"/>
+      <c r="D21" s="5"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1">
-      <c r="A22" s="10">
+      <c r="F21" s="13"/>
+      <c r="I21" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18" customHeight="1">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18" customHeight="1">
-      <c r="A23" s="10">
+    <row r="23" spans="1:9" ht="18" customHeight="1">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="6"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" ht="18" customHeight="1">
-      <c r="A24" s="10">
+      <c r="F23" s="13"/>
+      <c r="I23" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18" customHeight="1">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>86</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F24" s="11"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18" customHeight="1">
-      <c r="A25" s="10">
+    <row r="25" spans="1:9" ht="18" customHeight="1">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="6"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" ht="18" customHeight="1">
-      <c r="A26" s="10">
+      <c r="F25" s="13"/>
+      <c r="I25" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18" customHeight="1">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="11"/>
-    </row>
-    <row r="27" spans="1:7" ht="18" customHeight="1">
-      <c r="A27" s="10">
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" ht="18" customHeight="1">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1">
-      <c r="A28" s="10">
+      <c r="I27" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18" customHeight="1">
+      <c r="A28" s="9">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="6"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" spans="1:7" ht="18" customHeight="1">
-      <c r="A29" s="10">
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" ht="18" customHeight="1">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="6"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" ht="18" customHeight="1">
-      <c r="A30" s="10">
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" customHeight="1">
+      <c r="A30" s="9">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="6"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1">
+      <c r="F30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" customHeight="1">
       <c r="G31" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="18" customHeight="1">
+    <row r="32" spans="1:9" ht="18" customHeight="1">
       <c r="G32" s="3" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
update syllabus to move back homework 3
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29540" yWindow="9100" windowWidth="23220" windowHeight="17700" tabRatio="793"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="793"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -451,8 +451,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="137">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -635,7 +637,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="137">
+  <cellStyles count="139">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -704,6 +706,7 @@
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -772,6 +775,7 @@
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1107,7 +1111,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1365,19 +1369,20 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
-      <c r="A14" s="9">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1">
       <c r="A15" s="9">
@@ -1426,9 +1431,6 @@
       <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="E17" s="5" t="s">
         <v>91</v>
       </c>
@@ -1446,6 +1448,9 @@
       </c>
       <c r="C18" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="10"/>

</xml_diff>

<commit_message>
syllabus updates for generator topics and homework makeup assignments
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="793"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="107">
   <si>
     <t>Date</t>
   </si>
@@ -63,18 +63,12 @@
     <t>Lighting Practice</t>
   </si>
   <si>
-    <t>Electromagnetic Physics</t>
-  </si>
-  <si>
     <t>Motors</t>
   </si>
   <si>
     <t>Motor Systems</t>
   </si>
   <si>
-    <t>Utility Grid Technology</t>
-  </si>
-  <si>
     <t>Time Value of Money</t>
   </si>
   <si>
@@ -312,9 +306,6 @@
     <t>Quiz 4</t>
   </si>
   <si>
-    <t>Quiz 5</t>
-  </si>
-  <si>
     <t>Quiz 6</t>
   </si>
   <si>
@@ -340,6 +331,18 @@
   </si>
   <si>
     <t>HWM1-3</t>
+  </si>
+  <si>
+    <t>Generator Physics</t>
+  </si>
+  <si>
+    <t>Generator and Grid Technology</t>
+  </si>
+  <si>
+    <t>HWM 4</t>
+  </si>
+  <si>
+    <t>HWM 5</t>
   </si>
 </sst>
 </file>
@@ -448,8 +451,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -662,7 +667,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="169">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -746,6 +751,7 @@
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -829,6 +835,7 @@
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1163,15 +1170,15 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -1184,13 +1191,13 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>1</v>
@@ -1202,10 +1209,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1">
@@ -1213,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -1227,7 +1234,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>8</v>
@@ -1241,20 +1248,20 @@
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1">
@@ -1262,16 +1269,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="14"/>
       <c r="G5" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1">
@@ -1279,18 +1286,18 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1">
@@ -1298,18 +1305,18 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1">
@@ -1317,18 +1324,18 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="14"/>
       <c r="G8" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1">
@@ -1336,10 +1343,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -1350,14 +1357,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F10" s="14"/>
     </row>
@@ -1366,18 +1373,18 @@
         <v>10</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F11" s="14"/>
       <c r="I11" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1">
@@ -1385,20 +1392,20 @@
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1">
@@ -1406,7 +1413,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>9</v>
@@ -1415,10 +1422,10 @@
       <c r="E13" s="12"/>
       <c r="F13" s="14"/>
       <c r="G13" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1">
@@ -1426,138 +1433,140 @@
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1">
-      <c r="A15" s="9">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18" customHeight="1">
+      <c r="A16" s="11">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" customHeight="1">
+      <c r="A17" s="11">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
+      <c r="C17" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="I17" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" customHeight="1">
+      <c r="A18" s="11">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:9" ht="18" customHeight="1">
+      <c r="A19" s="11">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="4" t="s">
+    </row>
+    <row r="20" spans="1:9" ht="18" customHeight="1">
+      <c r="A20" s="11">
+        <v>6</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18" customHeight="1">
+      <c r="A21" s="11">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="14"/>
+      <c r="I21" s="4" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="18" customHeight="1">
-      <c r="A16" s="9">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="18" customHeight="1">
-      <c r="A17" s="9">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="I17" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="18" customHeight="1">
-      <c r="A18" s="9">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:9" ht="18" customHeight="1">
-      <c r="A19" s="9">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="18" customHeight="1">
-      <c r="A20" s="9">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="18" customHeight="1">
-      <c r="A21" s="9">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="10"/>
-      <c r="I21" s="4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1">
@@ -1565,14 +1574,14 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1">
@@ -1580,20 +1589,20 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>13</v>
+        <v>103</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1">
@@ -1601,13 +1610,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F24" s="10"/>
     </row>
@@ -1616,18 +1625,18 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="10"/>
       <c r="I25" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1">
@@ -1635,13 +1644,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="10"/>
@@ -1651,17 +1660,17 @@
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1">
@@ -1669,12 +1678,14 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>105</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="10"/>
     </row>
@@ -1683,12 +1694,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="10"/>
     </row>
@@ -1697,7 +1710,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>7</v>
@@ -1708,17 +1721,17 @@
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1">
       <c r="G31" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1">
       <c r="G32" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="7:7" ht="18" customHeight="1">
       <c r="G33" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moves due date on final report
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="793"/>
@@ -451,8 +451,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -667,7 +669,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="171">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -752,6 +754,7 @@
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -836,6 +839,7 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1170,8 +1174,8 @@
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1570,34 +1574,36 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1">
-      <c r="A22" s="9">
+      <c r="A22" s="11">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="10" t="s">
+      <c r="D22" s="13"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1">
-      <c r="A23" s="9">
+      <c r="A23" s="11">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="10"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="5" t="s">
         <v>74</v>
       </c>
@@ -1666,9 +1672,7 @@
         <v>73</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="F27" s="10"/>
       <c r="I27" s="4" t="s">
         <v>97</v>
       </c>
@@ -1687,7 +1691,9 @@
         <v>105</v>
       </c>
       <c r="E28" s="5"/>
-      <c r="F28" s="10"/>
+      <c r="F28" s="10" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1">
       <c r="A29" s="9">
@@ -1737,7 +1743,7 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
-  <pageSetup scale="79" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
updates syllabus with final exam and HW5M due date
</commit_message>
<xml_diff>
--- a/syllabus/338-syllabus.xlsx
+++ b/syllabus/338-syllabus.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="793"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -343,6 +343,12 @@
   </si>
   <si>
     <t>HWM 5</t>
+  </si>
+  <si>
+    <t>Final Exam</t>
+  </si>
+  <si>
+    <t>Mon 08 Dec 2014</t>
   </si>
 </sst>
 </file>
@@ -451,8 +457,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="171">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -669,7 +677,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="171">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -755,6 +763,7 @@
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -840,6 +849,7 @@
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1175,7 +1185,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
@@ -1705,9 +1715,7 @@
       <c r="C29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>106</v>
-      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="10"/>
     </row>
@@ -1726,6 +1734,18 @@
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>106</v>
+      </c>
       <c r="G31" s="3" t="s">
         <v>75</v>
       </c>

</xml_diff>